<commit_message>
add food type in this
</commit_message>
<xml_diff>
--- a/public/assets/products sample.xlsx
+++ b/public/assets/products sample.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">description</t>
   </si>
   <si>
-    <t xml:space="preserve">sss</t>
+    <t xml:space="preserve">food Type (halal/haram)</t>
   </si>
 </sst>
 </file>
@@ -170,10 +170,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -182,13 +182,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
@@ -226,7 +227,9 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G2" s="2"/>
@@ -242,11 +245,6 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G6" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H11" s="0" t="s">
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
add more feild in product
</commit_message>
<xml_diff>
--- a/public/assets/products sample.xlsx
+++ b/public/assets/products sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -28,13 +28,19 @@
     <t xml:space="preserve">code</t>
   </si>
   <si>
+    <t xml:space="preserve">tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand</t>
+  </si>
+  <si>
     <t xml:space="preserve">category</t>
   </si>
   <si>
     <t xml:space="preserve">sub_category</t>
   </si>
   <si>
-    <t xml:space="preserve">tags</t>
+    <t xml:space="preserve">Purchase Price</t>
   </si>
   <si>
     <t xml:space="preserve">rate</t>
@@ -47,6 +53,15 @@
   </si>
   <si>
     <t xml:space="preserve">quantity_alert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image (URL)</t>
   </si>
   <si>
     <t xml:space="preserve">status (active / un-active)</t>
@@ -63,7 +78,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -93,6 +108,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,12 +159,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -167,27 +193,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="4.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="5.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="25.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -197,7 +227,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -224,22 +254,31 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G3" s="2"/>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G4" s="2"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G5" s="2"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G6" s="2"/>
+      <c r="I6" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
add new field unit type
</commit_message>
<xml_diff>
--- a/public/assets/products sample.xlsx
+++ b/public/assets/products sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Muhammad Nasir\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\Horeca-admin\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB03B1E-8A81-4A90-BEC7-A1430146DF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9656B539-23B1-4915-9A2B-6844ED835AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Package quantity</t>
+  </si>
+  <si>
+    <t>Unit  Type</t>
   </si>
 </sst>
 </file>
@@ -501,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,9 +532,10 @@
     <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -595,8 +599,11 @@
       <c r="U1" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="V1" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2121</v>
       </c>
@@ -659,6 +666,9 @@
       </c>
       <c r="U2">
         <v>11</v>
+      </c>
+      <c r="V2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>